<commit_message>
Tela de Checkout concluída
</commit_message>
<xml_diff>
--- a/Documentos/Estimativa de Projeto/ESTIMATIVA.xlsx
+++ b/Documentos/Estimativa de Projeto/ESTIMATIVA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BrenoXDMoon\Documents\GitHub\ProjetoLes\Documentos\Estimativa de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847E2020-F21E-476E-B468-D4552F720172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60EC19B-9576-4B9A-A7AA-333DF0028B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9FF7230-91BA-A544-8A5A-3054F2DD43A9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
   <si>
     <t>(horas)</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Tela de Alteração de Cliente</t>
-  </si>
-  <si>
     <t>Inativar cadastro de cliente</t>
   </si>
   <si>
@@ -206,12 +203,6 @@
     <t>Tela de Cadastro de Carta</t>
   </si>
   <si>
-    <t>Tela de Consulta de Carta</t>
-  </si>
-  <si>
-    <t>Tela de Alteração de Carta</t>
-  </si>
-  <si>
     <t>Selecionar cartão de pagamento</t>
   </si>
   <si>
@@ -221,10 +212,70 @@
     <t>Em Andamento</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
     <t>Não iniciado</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>Tela de Edição de Carta</t>
+  </si>
+  <si>
+    <t>Tela de Edição de Cliente</t>
+  </si>
+  <si>
+    <t>Tela de Cadastro de Endereço</t>
+  </si>
+  <si>
+    <t>Tela de Edição de Endereço</t>
+  </si>
+  <si>
+    <t>Tela de Cadastro de Documento</t>
+  </si>
+  <si>
+    <t>Tela de Edição de Documento</t>
+  </si>
+  <si>
+    <t>Tela de Cadastro de Cartão de Crédito</t>
+  </si>
+  <si>
+    <t>Tela de Edição de Cartão de Crédito</t>
+  </si>
+  <si>
+    <t>Tela de Perfil de Cliente</t>
+  </si>
+  <si>
+    <t>Tela de Edição apenas da Senha do Cliente</t>
+  </si>
+  <si>
+    <t>Tela de Edição dos Dados Básicos de Cliente</t>
+  </si>
+  <si>
+    <t>Tela de Cadastro de Cupom</t>
+  </si>
+  <si>
+    <t>Tela de Consulta de Cupom</t>
+  </si>
+  <si>
+    <t>Tela de Edição de Cupom</t>
+  </si>
+  <si>
+    <t>Tela de Consulta de Carta (Admin)</t>
+  </si>
+  <si>
+    <t>Tela de Consulta de Carta (Cliente)</t>
+  </si>
+  <si>
+    <t>Nesta tela é possível Excluir Cartas</t>
+  </si>
+  <si>
+    <t>Nesta tela é possível Excluir Cupons</t>
+  </si>
+  <si>
+    <t>Tela para Alterar Status de Pedido</t>
+  </si>
+  <si>
+    <t>Nesta tela serão listados os Endereços, Documentos, Cartões, Cupons de troca Disponíveis e Pedidos do Cliente, também contando com a possibilidade de Alterar apenas as senhas, Alterar dados do cliente e Excluir Cartões, Documentos e Endereços do cliente.</t>
   </si>
 </sst>
 </file>
@@ -298,6 +349,7 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,18 +382,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -380,12 +431,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -454,232 +506,29 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ruim" xfId="3" builtinId="27"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1236,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B692412-8401-4F44-8DDD-33476696CC96}">
-  <dimension ref="A1:U58"/>
+  <dimension ref="A1:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39:J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1099,7 @@
     <col min="6" max="6" width="3" style="1" customWidth="1"/>
     <col min="7" max="7" width="2.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="3" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.25" style="4" customWidth="1"/>
+    <col min="9" max="9" width="40.125" style="4" customWidth="1"/>
     <col min="10" max="10" width="14.75" style="3" customWidth="1"/>
     <col min="11" max="16384" width="10.875" style="3"/>
   </cols>
@@ -1290,11 +1139,11 @@
       <c r="E2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1345,8 +1194,8 @@
         <v>3</v>
       </c>
       <c r="I4" s="21"/>
-      <c r="J4" s="25" t="s">
-        <v>62</v>
+      <c r="J4" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1369,14 +1218,14 @@
         <v>3</v>
       </c>
       <c r="I5" s="21"/>
-      <c r="J5" s="25" t="s">
-        <v>62</v>
+      <c r="J5" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="19">
         <v>1</v>
@@ -1394,13 +1243,13 @@
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="19">
         <v>1</v>
@@ -1418,13 +1267,13 @@
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
@@ -1442,13 +1291,13 @@
       <c r="H8" s="19"/>
       <c r="I8" s="21"/>
       <c r="J8" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
@@ -1466,13 +1315,13 @@
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="19">
         <v>2</v>
@@ -1490,13 +1339,13 @@
       <c r="H10" s="19"/>
       <c r="I10" s="21"/>
       <c r="J10" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="19">
         <v>1</v>
@@ -1514,7 +1363,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="21"/>
       <c r="J11" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1537,8 +1386,8 @@
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="25" t="s">
-        <v>62</v>
+      <c r="J12" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1562,13 +1411,13 @@
       <c r="H13" s="19"/>
       <c r="I13" s="21"/>
       <c r="J13" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="19">
         <v>1</v>
@@ -1586,13 +1435,13 @@
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="19">
         <v>1</v>
@@ -1610,13 +1459,13 @@
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="19">
         <v>3</v>
@@ -1634,13 +1483,13 @@
       <c r="H16" s="19"/>
       <c r="I16" s="21"/>
       <c r="J16" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="19">
         <v>2</v>
@@ -1658,13 +1507,13 @@
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="19">
         <v>2</v>
@@ -1682,13 +1531,13 @@
       </c>
       <c r="I18" s="21"/>
       <c r="J18" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="19">
         <v>1</v>
@@ -1706,13 +1555,13 @@
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="19">
         <v>4</v>
@@ -1729,14 +1578,14 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="21"/>
-      <c r="J20" s="26" t="s">
-        <v>63</v>
+      <c r="J20" s="24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="19">
         <v>2</v>
@@ -1753,17 +1602,17 @@
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="21"/>
-      <c r="J21" s="26" t="s">
-        <v>63</v>
+      <c r="J21" s="28" t="s">
+        <v>59</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="19">
         <v>4</v>
@@ -1780,14 +1629,14 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="26" t="s">
-        <v>63</v>
+      <c r="J22" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="19">
         <v>2</v>
@@ -1804,14 +1653,14 @@
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="26" t="s">
-        <v>63</v>
+      <c r="J23" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="19">
         <v>1</v>
@@ -1828,14 +1677,14 @@
         <v>3</v>
       </c>
       <c r="I24" s="21"/>
-      <c r="J24" s="26" t="s">
-        <v>63</v>
+      <c r="J24" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" s="19">
         <v>1</v>
@@ -1852,14 +1701,14 @@
         <v>3</v>
       </c>
       <c r="I25" s="21"/>
-      <c r="J25" s="26" t="s">
-        <v>63</v>
+      <c r="J25" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="19">
         <v>2</v>
@@ -1876,14 +1725,14 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
       <c r="I26" s="21"/>
-      <c r="J26" s="26" t="s">
-        <v>63</v>
+      <c r="J26" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C27" s="19">
         <v>1</v>
@@ -1900,14 +1749,14 @@
       </c>
       <c r="H27" s="19"/>
       <c r="I27" s="21"/>
-      <c r="J27" s="26" t="s">
-        <v>63</v>
+      <c r="J27" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="19">
         <v>4</v>
@@ -1924,14 +1773,14 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
       <c r="I28" s="21"/>
-      <c r="J28" s="26" t="s">
-        <v>63</v>
+      <c r="J28" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="19">
         <v>4</v>
@@ -1948,14 +1797,14 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="26" t="s">
-        <v>63</v>
+      <c r="J29" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
       <c r="B30" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="19">
         <v>2</v>
@@ -1972,14 +1821,14 @@
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="26" t="s">
-        <v>63</v>
+      <c r="J30" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
       <c r="B31" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="19">
         <v>4</v>
@@ -1996,14 +1845,14 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="26" t="s">
-        <v>63</v>
+      <c r="J31" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
       <c r="B32" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="19">
         <v>4</v>
@@ -2020,14 +1869,14 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
       <c r="I32" s="21"/>
-      <c r="J32" s="26" t="s">
-        <v>63</v>
+      <c r="J32" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
       <c r="B33" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="19">
         <v>1</v>
@@ -2044,14 +1893,14 @@
         <v>3</v>
       </c>
       <c r="I33" s="21"/>
-      <c r="J33" s="26" t="s">
-        <v>63</v>
+      <c r="J33" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>
       <c r="B34" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="19">
         <v>2</v>
@@ -2068,14 +1917,14 @@
         <v>3</v>
       </c>
       <c r="I34" s="21"/>
-      <c r="J34" s="26" t="s">
-        <v>63</v>
+      <c r="J34" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
       <c r="B35" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="19">
         <v>3</v>
@@ -2092,14 +1941,14 @@
       </c>
       <c r="H35" s="19"/>
       <c r="I35" s="21"/>
-      <c r="J35" s="26" t="s">
-        <v>63</v>
+      <c r="J35" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="19">
         <v>3</v>
@@ -2116,14 +1965,14 @@
       </c>
       <c r="H36" s="19"/>
       <c r="I36" s="21"/>
-      <c r="J36" s="26" t="s">
-        <v>63</v>
+      <c r="J36" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="19">
         <v>4</v>
@@ -2140,8 +1989,8 @@
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
       <c r="I37" s="21"/>
-      <c r="J37" s="26" t="s">
-        <v>63</v>
+      <c r="J37" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2161,7 +2010,7 @@
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="19">
         <v>2</v>
@@ -2178,14 +2027,14 @@
       </c>
       <c r="H39" s="19"/>
       <c r="I39" s="21"/>
-      <c r="J39" s="25" t="s">
-        <v>61</v>
+      <c r="J39" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="22" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="C40" s="19">
         <v>2</v>
@@ -2201,39 +2050,35 @@
         <v>2</v>
       </c>
       <c r="H40" s="19"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="25" t="s">
-        <v>61</v>
+      <c r="I40" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
       <c r="B41" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="19">
-        <v>2</v>
-      </c>
-      <c r="D41" s="19">
-        <v>3</v>
-      </c>
-      <c r="E41" s="19">
-        <v>4</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19" t="s">
         <v>2</v>
       </c>
       <c r="H41" s="19"/>
       <c r="I41" s="21"/>
-      <c r="J41" s="25" t="s">
-        <v>61</v>
+      <c r="J41" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
       <c r="B42" s="22" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C42" s="19">
         <v>2</v>
@@ -2250,14 +2095,14 @@
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="21"/>
-      <c r="J42" s="25" t="s">
-        <v>61</v>
+      <c r="J42" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="20"/>
       <c r="B43" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C43" s="19">
         <v>2</v>
@@ -2274,14 +2119,14 @@
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="21"/>
-      <c r="J43" s="25" t="s">
-        <v>61</v>
+      <c r="J43" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="20"/>
       <c r="B44" s="22" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C44" s="19">
         <v>2</v>
@@ -2298,14 +2143,14 @@
       </c>
       <c r="H44" s="19"/>
       <c r="I44" s="21"/>
-      <c r="J44" s="25" t="s">
-        <v>61</v>
+      <c r="J44" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
       <c r="B45" s="22" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C45" s="19">
         <v>2</v>
@@ -2322,14 +2167,14 @@
       </c>
       <c r="H45" s="19"/>
       <c r="I45" s="21"/>
-      <c r="J45" s="25" t="s">
-        <v>61</v>
+      <c r="J45" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="20"/>
       <c r="B46" s="22" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C46" s="19">
         <v>2</v>
@@ -2346,14 +2191,14 @@
       </c>
       <c r="H46" s="19"/>
       <c r="I46" s="21"/>
-      <c r="J46" s="25" t="s">
-        <v>61</v>
+      <c r="J46" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
       <c r="B47" s="22" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C47" s="19">
         <v>2</v>
@@ -2370,14 +2215,14 @@
       </c>
       <c r="H47" s="19"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="25" t="s">
-        <v>61</v>
+      <c r="J47" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
       <c r="B48" s="22" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C48" s="19">
         <v>2</v>
@@ -2394,14 +2239,14 @@
       </c>
       <c r="H48" s="19"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="25" t="s">
-        <v>61</v>
+      <c r="J48" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="20"/>
       <c r="B49" s="22" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C49" s="19">
         <v>2</v>
@@ -2418,14 +2263,14 @@
       </c>
       <c r="H49" s="19"/>
       <c r="I49" s="21"/>
-      <c r="J49" s="25" t="s">
-        <v>61</v>
+      <c r="J49" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="20"/>
       <c r="B50" s="22" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C50" s="19">
         <v>2</v>
@@ -2442,14 +2287,14 @@
       </c>
       <c r="H50" s="19"/>
       <c r="I50" s="21"/>
-      <c r="J50" s="25" t="s">
-        <v>61</v>
+      <c r="J50" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="20"/>
       <c r="B51" s="22" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C51" s="19">
         <v>2</v>
@@ -2466,53 +2311,371 @@
       </c>
       <c r="H51" s="19"/>
       <c r="I51" s="21"/>
-      <c r="J51" s="25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="C52" s="14">
-        <f>SUM(C4:C51)</f>
-        <v>99</v>
-      </c>
-      <c r="D52" s="10">
-        <f>SUM(D4:D51)</f>
-        <v>159</v>
-      </c>
-      <c r="E52" s="13">
-        <f>SUM(E4:E51)</f>
-        <v>229</v>
-      </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="11"/>
+      <c r="J51" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="20"/>
+      <c r="B52" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="19">
+        <v>2</v>
+      </c>
+      <c r="D52" s="19">
+        <v>3</v>
+      </c>
+      <c r="E52" s="19">
+        <v>4</v>
+      </c>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="J52" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
+      <c r="B53" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="19">
+        <v>2</v>
+      </c>
+      <c r="D53" s="19">
+        <v>3</v>
+      </c>
+      <c r="E53" s="19">
+        <v>4</v>
+      </c>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="19">
+        <v>2</v>
+      </c>
+      <c r="D54" s="19">
+        <v>3</v>
+      </c>
+      <c r="E54" s="19">
+        <v>4</v>
+      </c>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="12"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="19">
+        <v>2</v>
+      </c>
+      <c r="D55" s="19">
+        <v>3</v>
+      </c>
+      <c r="E55" s="19">
+        <v>4</v>
+      </c>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="12"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="19">
+        <v>2</v>
+      </c>
+      <c r="D56" s="19">
+        <v>3</v>
+      </c>
+      <c r="E56" s="19">
+        <v>4</v>
+      </c>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J56" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="12"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" s="19">
+        <v>2</v>
+      </c>
+      <c r="D57" s="19">
+        <v>3</v>
+      </c>
+      <c r="E57" s="19">
+        <v>4</v>
+      </c>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="12"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="19">
+        <v>2</v>
+      </c>
+      <c r="D58" s="19">
+        <v>3</v>
+      </c>
+      <c r="E58" s="19">
+        <v>4</v>
+      </c>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H58" s="19"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="20"/>
+      <c r="B59" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="19">
+        <v>2</v>
+      </c>
+      <c r="D59" s="19">
+        <v>3</v>
+      </c>
+      <c r="E59" s="19">
+        <v>4</v>
+      </c>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H59" s="19"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="20"/>
+      <c r="B60" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="19">
+        <v>2</v>
+      </c>
+      <c r="D60" s="19">
+        <v>3</v>
+      </c>
+      <c r="E60" s="19">
+        <v>4</v>
+      </c>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H60" s="19"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+      <c r="B61" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="24"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="20"/>
+      <c r="B62" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="19">
+        <v>2</v>
+      </c>
+      <c r="D62" s="19">
+        <v>3</v>
+      </c>
+      <c r="E62" s="19">
+        <v>4</v>
+      </c>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H62" s="19"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="20"/>
+      <c r="B63" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="19">
+        <v>2</v>
+      </c>
+      <c r="D63" s="19">
+        <v>3</v>
+      </c>
+      <c r="E63" s="19">
+        <v>4</v>
+      </c>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H63" s="19"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="20"/>
+      <c r="B64" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="19">
+        <v>2</v>
+      </c>
+      <c r="D64" s="19">
+        <v>3</v>
+      </c>
+      <c r="E64" s="19">
+        <v>4</v>
+      </c>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H64" s="19"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="20"/>
+      <c r="B65" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" s="19">
+        <v>2</v>
+      </c>
+      <c r="D65" s="19">
+        <v>3</v>
+      </c>
+      <c r="E65" s="19">
+        <v>4</v>
+      </c>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H65" s="19"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+      <c r="C66" s="14">
+        <f>SUM(C4:C65)</f>
+        <v>123</v>
+      </c>
+      <c r="D66" s="10">
+        <f>SUM(D4:D65)</f>
+        <v>195</v>
+      </c>
+      <c r="E66" s="13">
+        <f>SUM(E4:E65)</f>
+        <v>277</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="11"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="12"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="12"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="12"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2:H3 F1 H1 F52:H1048576 H39:H51 F39:F51 H10:H37 F4:G37">
-    <cfRule type="containsText" dxfId="44" priority="94" operator="containsText" text=":)">
+  <conditionalFormatting sqref="F2:H3 F1 H1 H10:H37 F4:G37 F39:H1048576">
+    <cfRule type="containsText" dxfId="23" priority="94" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="95" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="22" priority="95" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="96" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="21" priority="96" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2527,13 +2690,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38:H38">
-    <cfRule type="containsText" dxfId="41" priority="87" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="20" priority="87" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",F38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="88" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="19" priority="88" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",F38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="89" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="18" priority="89" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",F38)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2548,68 +2711,57 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="38" priority="79" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="17" priority="79" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",H8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="80" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="16" priority="80" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",H8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="81" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="15" priority="81" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="containsText" dxfId="35" priority="73" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="14" priority="73" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="74" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="13" priority="74" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="75" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="12" priority="75" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G39:G51">
-    <cfRule type="containsText" dxfId="32" priority="55" operator="containsText" text=":)">
-      <formula>NOT(ISERROR(SEARCH(":)",G39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="56" operator="containsText" text=":|">
-      <formula>NOT(ISERROR(SEARCH(":|",G39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="57" operator="containsText" text=":(">
-      <formula>NOT(ISERROR(SEARCH(":(",G39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H4:H7">
-    <cfRule type="containsText" dxfId="29" priority="22" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="11" priority="22" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="10" priority="23" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="9" priority="24" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="8" priority="19" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="7" priority="20" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="6" priority="21" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3 T3">
-    <cfRule type="containsText" dxfId="23" priority="16" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="5" priority="16" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",R3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="4" priority="17" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",R3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="3" priority="18" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",R3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2624,13 +2776,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text=":)">
+    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text=":)">
       <formula>NOT(ISERROR(SEARCH(":)",S3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text=":|">
+    <cfRule type="containsText" dxfId="1" priority="13" operator="containsText" text=":|">
       <formula>NOT(ISERROR(SEARCH(":|",S3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text=":(">
+    <cfRule type="containsText" dxfId="0" priority="14" operator="containsText" text=":(">
       <formula>NOT(ISERROR(SEARCH(":(",S3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2640,23 +2792,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="13526e60-2309-4b29-b958-df71ed96cd48" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100301B24C317AEAA4A9E81584B0F1753BF" ma:contentTypeVersion="1" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ea2d69a61fc7a42705a79b5983b790a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="13526e60-2309-4b29-b958-df71ed96cd48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0df65a6dff0c15483f5753a509519d7a" ns2:_="">
     <xsd:import namespace="13526e60-2309-4b29-b958-df71ed96cd48"/>
@@ -2782,25 +2917,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C51C229-CA01-440E-B2BE-F6F69B7DA214}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="13526e60-2309-4b29-b958-df71ed96cd48"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A55BC6FF-54C9-4DD8-8203-E7CA3890AFA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="13526e60-2309-4b29-b958-df71ed96cd48" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAA58E31-EA10-4926-9E03-5E76E8F2B1AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2816,4 +2950,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A55BC6FF-54C9-4DD8-8203-E7CA3890AFA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C51C229-CA01-440E-B2BE-F6F69B7DA214}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="13526e60-2309-4b29-b958-df71ed96cd48"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>